<commit_message>
Added EBIT, EBITA, restructure Taxes, fix layout and print
</commit_message>
<xml_diff>
--- a/assumptions.xlsx
+++ b/assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/development/python/financial-statements-projections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0414258-D52D-164F-83D1-CC647BF51553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE1B118-BF3F-5F46-BFCD-958B9721FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1300" windowWidth="34860" windowHeight="19420" activeTab="1" xr2:uid="{9D650151-92C7-924A-9CDF-D8A9F0818C4B}"/>
+    <workbookView xWindow="1620" yWindow="1300" windowWidth="34860" windowHeight="19420" xr2:uid="{9D650151-92C7-924A-9CDF-D8A9F0818C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>Inflation Rate</t>
   </si>
   <si>
-    <t>Tax Rate (%)</t>
-  </si>
-  <si>
     <t>Operations</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Revenue</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705F41C1-1485-AC40-A5F3-45ECB1240822}">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -820,7 +820,7 @@
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -849,7 +849,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="16">
         <v>0.1</v>
@@ -889,10 +889,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="16">
-        <v>2.9999999999999995E-2</v>
+        <v>0.12</v>
       </c>
       <c r="C4" s="18">
         <v>0.22399907615426834</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="16">
-        <v>1.4196369997813252</v>
+        <v>0.12</v>
       </c>
       <c r="C5" s="16">
         <v>0.17022623742379844</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="19" t="str">
         <f t="shared" ref="C6:L6" si="0">B6</f>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="8" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="19">
         <v>0.02</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="19">
         <v>0.9</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="19">
         <v>0</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="19">
         <v>0</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="19">
         <v>0</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="19">
         <v>0</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="20" t="str">
         <f t="shared" ref="B15" si="3">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="19">
         <v>0</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="19">
         <v>0</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="22">
         <v>0</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="24">
         <v>0.1</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="25">
         <v>0</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="25">
         <v>0</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B29" s="16">
         <v>0.3</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -2310,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F6569-4898-7840-9C35-A7AF6E8E1336}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2318,7 +2318,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7">
         <v>2025</v>
@@ -2356,7 +2356,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="26">
         <v>10000</v>

</xml_diff>

<commit_message>
Finish P&L and Balance Sheet Current Assets and it's components
</commit_message>
<xml_diff>
--- a/assumptions.xlsx
+++ b/assumptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/development/python/financial-statements-projections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE1B118-BF3F-5F46-BFCD-958B9721FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9DE2FC-3017-7F45-A80B-6BFDFE5BDEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1300" windowWidth="34860" windowHeight="19420" xr2:uid="{9D650151-92C7-924A-9CDF-D8A9F0818C4B}"/>
+    <workbookView xWindow="1620" yWindow="1300" windowWidth="34860" windowHeight="19420" activeTab="1" xr2:uid="{9D650151-92C7-924A-9CDF-D8A9F0818C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>roberto.serrano</author>
   </authors>
   <commentList>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{996C2549-49B6-B341-8ED0-BDEB02F94F32}">
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{996C2549-49B6-B341-8ED0-BDEB02F94F32}">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{7F64E016-0907-8E4C-B008-61E062381203}">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{7F64E016-0907-8E4C-B008-61E062381203}">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Assumption</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Operations</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Working Capital/Revenues</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>Other Current Liabilities</t>
   </si>
   <si>
-    <t>Net Working Capital</t>
-  </si>
-  <si>
     <t>1: CapX/Revs    (Input, Mode 1)</t>
   </si>
   <si>
@@ -239,6 +233,15 @@
   </si>
   <si>
     <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Other Oper Inc/Exp</t>
+  </si>
+  <si>
+    <t>Other Ratios</t>
+  </si>
+  <si>
+    <t>Working Capital</t>
   </si>
 </sst>
 </file>
@@ -769,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705F41C1-1485-AC40-A5F3-45ECB1240822}">
-  <dimension ref="A1:Y60"/>
+  <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +852,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="16">
         <v>0.1</v>
@@ -889,7 +892,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="16">
         <v>0.12</v>
@@ -930,7 +933,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="16">
         <v>0.12</v>
@@ -971,50 +974,50 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="19" t="str">
+        <v>11</v>
+      </c>
+      <c r="B6" s="19">
+        <v>0</v>
+      </c>
+      <c r="C6" s="19">
         <f t="shared" ref="C6:L6" si="0">B6</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="F6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="I6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="J6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="J6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="K6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="K6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="L6" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>0</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -1036,7 +1039,7 @@
     </row>
     <row r="8" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1054,7 +1057,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="19">
         <v>0.02</v>
@@ -1104,7 +1107,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="19">
         <v>0.9</v>
@@ -1153,7 +1156,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="19">
         <v>0</v>
@@ -1203,7 +1206,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="19">
         <v>0</v>
@@ -1253,7 +1256,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="19">
         <v>0</v>
@@ -1303,7 +1306,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="19">
         <v>0</v>
@@ -1352,58 +1355,25 @@
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="20" t="str">
-        <f t="shared" ref="B15" si="3">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="C15" s="20" t="str">
-        <f t="shared" ref="C15" si="4">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="D15" s="20" t="str">
-        <f t="shared" ref="D15" si="5">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="E15" s="20" t="str">
-        <f t="shared" ref="E15" si="6">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="F15" s="20" t="str">
-        <f t="shared" ref="F15" si="7">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="G15" s="20" t="str">
-        <f t="shared" ref="G15" si="8">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="H15" s="20" t="str">
-        <f t="shared" ref="H15" si="9">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="I15" s="20" t="str">
-        <f t="shared" ref="I15" si="10">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="J15" s="20" t="str">
-        <f t="shared" ref="J15" si="11">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="K15" s="20" t="str">
-        <f t="shared" ref="K15" si="12">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="L15" s="20" t="str">
-        <f t="shared" ref="L15" si="13">IF(ISERROR(#REF!/#REF!),"N.A.",#REF!/#REF!)</f>
-        <v>N.A.</v>
-      </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
+      <c r="A16" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -1419,7 +1389,7 @@
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="11"/>
@@ -1438,67 +1408,99 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19">
+        <f t="shared" ref="C18:L19" si="3">B18</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="19">
         <v>0</v>
       </c>
       <c r="C19" s="19">
-        <f t="shared" ref="C19:L20" si="14">B19</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L19" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M19" s="2"/>
@@ -1506,199 +1508,190 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="19">
-        <v>0</v>
-      </c>
-      <c r="C20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="19">
-        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="22">
+        <v>0</v>
+      </c>
+      <c r="C20" s="23">
+        <v>472000</v>
+      </c>
+      <c r="D20" s="23">
+        <v>687000</v>
+      </c>
+      <c r="E20" s="23">
+        <v>550000</v>
+      </c>
+      <c r="F20" s="23">
+        <v>0</v>
+      </c>
+      <c r="G20" s="23">
+        <v>0</v>
+      </c>
+      <c r="H20" s="23">
+        <v>472000</v>
+      </c>
+      <c r="I20" s="23">
+        <v>687000</v>
+      </c>
+      <c r="J20" s="23">
+        <v>550000</v>
+      </c>
+      <c r="K20" s="23">
+        <v>0</v>
+      </c>
+      <c r="L20" s="23">
+        <f>K20</f>
         <v>0</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="24">
+        <v>0.66080000000000005</v>
+      </c>
+      <c r="D21" s="24">
+        <v>0.34377118644067794</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0.20643658326143227</v>
+      </c>
+      <c r="F21" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G21" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H21" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I21" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J21" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K21" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L21" s="24">
+        <f>K21</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="22">
-        <v>0</v>
-      </c>
-      <c r="C21" s="23">
-        <v>472000</v>
-      </c>
-      <c r="D21" s="23">
-        <v>687000</v>
-      </c>
-      <c r="E21" s="23">
-        <v>550000</v>
-      </c>
-      <c r="F21" s="23">
-        <v>0</v>
-      </c>
-      <c r="G21" s="23">
-        <v>0</v>
-      </c>
-      <c r="H21" s="23">
-        <v>472000</v>
-      </c>
-      <c r="I21" s="23">
-        <v>687000</v>
-      </c>
-      <c r="J21" s="23">
-        <v>550000</v>
-      </c>
-      <c r="K21" s="23">
-        <v>0</v>
-      </c>
-      <c r="L21" s="23">
-        <f>K21</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="C22" s="24">
-        <v>0.66080000000000005</v>
-      </c>
-      <c r="D22" s="24">
-        <v>0.34377118644067794</v>
-      </c>
-      <c r="E22" s="24">
-        <v>0.20643658326143227</v>
-      </c>
-      <c r="F22" s="24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G22" s="24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H22" s="24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I22" s="24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J22" s="24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K22" s="24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L22" s="24">
+      <c r="B22" s="19">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0</v>
+      </c>
+      <c r="D22" s="19">
+        <v>0</v>
+      </c>
+      <c r="E22" s="19">
+        <v>0</v>
+      </c>
+      <c r="F22" s="19">
+        <v>0</v>
+      </c>
+      <c r="G22" s="19">
+        <v>0</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0</v>
+      </c>
+      <c r="I22" s="19">
+        <v>0</v>
+      </c>
+      <c r="J22" s="19">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19">
         <f>K22</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="19">
-        <v>0</v>
-      </c>
-      <c r="C23" s="19">
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <v>0</v>
-      </c>
-      <c r="E23" s="19">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19">
-        <v>0</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="I23" s="19">
-        <v>0</v>
-      </c>
-      <c r="J23" s="19">
-        <v>0</v>
-      </c>
-      <c r="K23" s="19">
-        <v>0</v>
-      </c>
-      <c r="L23" s="19">
-        <f>K23</f>
-        <v>0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="25">
+        <v>0</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0</v>
+      </c>
+      <c r="D24" s="25">
+        <v>0</v>
+      </c>
+      <c r="E24" s="25">
+        <v>0</v>
+      </c>
+      <c r="F24" s="25">
+        <v>0</v>
+      </c>
+      <c r="G24" s="25">
+        <v>0</v>
+      </c>
+      <c r="H24" s="25">
+        <v>141600</v>
+      </c>
+      <c r="I24" s="25">
+        <v>206100</v>
+      </c>
+      <c r="J24" s="25">
+        <v>165000</v>
+      </c>
+      <c r="K24" s="25">
+        <v>0</v>
+      </c>
+      <c r="L24" s="25">
+        <f>K24</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="B25" s="25">
         <v>0</v>
       </c>
@@ -1718,13 +1711,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="25">
-        <v>141600</v>
+        <v>472000</v>
       </c>
       <c r="I25" s="25">
-        <v>206100</v>
+        <v>687000</v>
       </c>
       <c r="J25" s="25">
-        <v>165000</v>
+        <v>550000</v>
       </c>
       <c r="K25" s="25">
         <v>0</v>
@@ -1737,48 +1730,25 @@
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="25">
-        <v>0</v>
-      </c>
-      <c r="C26" s="25">
-        <v>0</v>
-      </c>
-      <c r="D26" s="25">
-        <v>0</v>
-      </c>
-      <c r="E26" s="25">
-        <v>0</v>
-      </c>
-      <c r="F26" s="25">
-        <v>0</v>
-      </c>
-      <c r="G26" s="25">
-        <v>0</v>
-      </c>
-      <c r="H26" s="25">
-        <v>472000</v>
-      </c>
-      <c r="I26" s="25">
-        <v>687000</v>
-      </c>
-      <c r="J26" s="25">
-        <v>550000</v>
-      </c>
-      <c r="K26" s="25">
-        <v>0</v>
-      </c>
-      <c r="L26" s="25">
-        <f>K26</f>
-        <v>0</v>
-      </c>
+      <c r="A26" s="11"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
+      <c r="A27" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
@@ -1794,60 +1764,55 @@
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="A28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C28" s="16">
+        <v>0.31</v>
+      </c>
+      <c r="D28" s="16">
+        <v>0.32</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="I28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="J28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="K28" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="L28" s="16">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="C29" s="16">
-        <v>0.31</v>
-      </c>
-      <c r="D29" s="16">
-        <v>0.32</v>
-      </c>
-      <c r="E29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="F29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="G29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="H29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="I29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="J29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="K29" s="16">
-        <v>0.33</v>
-      </c>
-      <c r="L29" s="16">
-        <v>0.33</v>
-      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="16"/>
@@ -1863,75 +1828,78 @@
       <c r="L30" s="16"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
+      <c r="A31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="C32" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D32" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="E32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L32" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="16">
-        <v>0.02</v>
-      </c>
-      <c r="C33" s="16">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D33" s="16">
-        <v>0.03</v>
-      </c>
-      <c r="E33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="I33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="J33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="K33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="L33" s="16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -1945,8 +1913,8 @@
       <c r="L34" s="15"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>8</v>
+      <c r="A35" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -1962,7 +1930,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -1978,7 +1946,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -1994,7 +1962,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2010,7 +1978,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2025,9 +1993,6 @@
       <c r="L39" s="15"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
@@ -2287,19 +2252,6 @@
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2308,17 +2260,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57F6569-4898-7840-9C35-A7AF6E8E1336}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="7">
         <v>2025</v>
@@ -2372,7 +2327,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="26">
         <v>10000</v>
@@ -2388,6 +2343,32 @@
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="26">
+        <v>5000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Accounts Payable and Other Current Liabilities to Current Liabilities
</commit_message>
<xml_diff>
--- a/assumptions.xlsx
+++ b/assumptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/development/python/financial-statements-projections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9DE2FC-3017-7F45-A80B-6BFDFE5BDEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D534B0-E263-0344-9747-4F00A7AA5954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="1300" windowWidth="34860" windowHeight="19420" activeTab="1" xr2:uid="{9D650151-92C7-924A-9CDF-D8A9F0818C4B}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Assumption</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>Other Ratios</t>
-  </si>
-  <si>
-    <t>Working Capital</t>
   </si>
 </sst>
 </file>
@@ -774,9 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705F41C1-1485-AC40-A5F3-45ECB1240822}">
   <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2263,7 +2258,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2356,18 +2351,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="26">
-        <v>5000</v>
-      </c>
+      <c r="B8" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Calculate Equity including Retained Earnings
</commit_message>
<xml_diff>
--- a/assumptions.xlsx
+++ b/assumptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/development/python/financial-statements-projections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D534B0-E263-0344-9747-4F00A7AA5954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FDDEAC-8A8F-2F42-8740-466D1A9F88EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="1300" windowWidth="34860" windowHeight="19420" activeTab="1" xr2:uid="{9D650151-92C7-924A-9CDF-D8A9F0818C4B}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Assumption</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Other Ratios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance Sheet </t>
+  </si>
+  <si>
+    <t>Common Stock and Paid in Capital</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -387,14 +393,11 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -408,9 +411,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -428,9 +428,8 @@
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="38" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -775,151 +774,151 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
         <v>2025</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="6">
         <v>2026</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="6">
         <v>2027</v>
       </c>
-      <c r="E1" s="7">
+      <c r="E1" s="6">
         <v>2028</v>
       </c>
-      <c r="F1" s="7">
+      <c r="F1" s="6">
         <v>2029</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1" s="6">
         <v>2030</v>
       </c>
-      <c r="H1" s="7">
+      <c r="H1" s="6">
         <v>2031</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="6">
         <v>2032</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J1" s="6">
         <v>2033</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K1" s="6">
         <v>2034</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="6">
         <v>2035</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>0.1</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="14">
         <v>0.1</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="14">
         <v>0.1</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="14">
         <v>0.1</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="14">
         <v>0.1</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="14">
         <v>0.1</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="14">
         <v>0.1</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="14">
         <v>0.1</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="14">
         <v>0.1</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="14">
         <v>0.1</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="14">
         <v>0.1</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>0.12</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.22399907615426834</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="14">
         <v>0.23935496262995173</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="14">
         <v>0.27627535210381698</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <v>0.35141704744232832</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="14">
         <v>0.45568645633144167</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="14">
         <v>0.45568645633144167</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="14">
         <v>0.45568645633144167</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="14">
         <v>0.45568645633144167</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="14">
         <v>0.45568645633144167</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="14">
         <f>K4</f>
         <v>0.45568645633144167</v>
       </c>
@@ -927,40 +926,40 @@
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="14">
         <v>0.12</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="14">
         <v>0.17022623742379844</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="14">
         <v>7.9275921549008074E-2</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="14">
         <v>6.5304797005743098E-2</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <v>8.5401581491282311E-2</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="14">
         <v>0.11310631119106347</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="14">
         <v>0.11310631119106347</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="14">
         <v>0.11310631119106347</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="14">
         <v>0.11310631119106347</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="14">
         <v>0.11310631119106347</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="14">
         <f>K5</f>
         <v>0.11310631119106347</v>
       </c>
@@ -968,49 +967,49 @@
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="19">
-        <v>0</v>
-      </c>
-      <c r="C6" s="19">
+      <c r="B6" s="17">
+        <v>0</v>
+      </c>
+      <c r="C6" s="17">
         <f t="shared" ref="C6:L6" si="0">B6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1018,82 +1017,82 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="17">
         <v>0.02</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="17">
         <f t="shared" ref="C9:L10" si="1">B9</f>
         <v>0.02</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
@@ -1101,48 +1100,48 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="17">
         <v>0.9</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="17">
         <v>0.1</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="17">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -1150,49 +1149,49 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="19">
-        <v>0</v>
-      </c>
-      <c r="C11" s="19">
+      <c r="B11" s="17">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17">
         <f t="shared" ref="C11:L14" si="2">B11</f>
         <v>0</v>
       </c>
-      <c r="D11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="19">
+      <c r="D11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1200,49 +1199,49 @@
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="19">
-        <v>0</v>
-      </c>
-      <c r="C12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="19">
+      <c r="B12" s="17">
+        <v>0</v>
+      </c>
+      <c r="C12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1250,49 +1249,49 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="19">
-        <v>0</v>
-      </c>
-      <c r="C13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="19">
+      <c r="B13" s="17">
+        <v>0</v>
+      </c>
+      <c r="C13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1300,49 +1299,49 @@
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="19">
-        <v>0</v>
-      </c>
-      <c r="C14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="19">
+      <c r="B14" s="17">
+        <v>0</v>
+      </c>
+      <c r="C14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1350,101 +1349,101 @@
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="19">
-        <v>0</v>
-      </c>
-      <c r="C18" s="19">
+      <c r="B18" s="17">
+        <v>0</v>
+      </c>
+      <c r="C18" s="17">
         <f t="shared" ref="C18:L19" si="3">B18</f>
         <v>0</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1452,49 +1451,49 @@
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="19">
+      <c r="B19" s="17">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -1502,40 +1501,40 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="22">
-        <v>0</v>
-      </c>
-      <c r="C20" s="23">
+      <c r="B20" s="20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21">
         <v>472000</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="21">
         <v>687000</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="21">
         <v>550000</v>
       </c>
-      <c r="F20" s="23">
-        <v>0</v>
-      </c>
-      <c r="G20" s="23">
-        <v>0</v>
-      </c>
-      <c r="H20" s="23">
+      <c r="F20" s="21">
+        <v>0</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0</v>
+      </c>
+      <c r="H20" s="21">
         <v>472000</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="21">
         <v>687000</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="21">
         <v>550000</v>
       </c>
-      <c r="K20" s="23">
-        <v>0</v>
-      </c>
-      <c r="L20" s="23">
+      <c r="K20" s="21">
+        <v>0</v>
+      </c>
+      <c r="L20" s="21">
         <f>K20</f>
         <v>0</v>
       </c>
@@ -1543,81 +1542,81 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="17">
         <v>0.1</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="17">
         <v>0.66080000000000005</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="17">
         <v>0.34377118644067794</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="17">
         <v>0.20643658326143227</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I21" s="24">
+      <c r="I21" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="17">
         <f>K21</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="19">
-        <v>0</v>
-      </c>
-      <c r="C22" s="19">
-        <v>0</v>
-      </c>
-      <c r="D22" s="19">
-        <v>0</v>
-      </c>
-      <c r="E22" s="19">
-        <v>0</v>
-      </c>
-      <c r="F22" s="19">
-        <v>0</v>
-      </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-      <c r="H22" s="19">
-        <v>0</v>
-      </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="19">
-        <v>0</v>
-      </c>
-      <c r="K22" s="19">
-        <v>0</v>
-      </c>
-      <c r="L22" s="19">
+      <c r="B22" s="17">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17">
+        <v>0</v>
+      </c>
+      <c r="D22" s="17">
+        <v>0</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0</v>
+      </c>
+      <c r="G22" s="17">
+        <v>0</v>
+      </c>
+      <c r="H22" s="17">
+        <v>0</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="17">
         <f>K22</f>
         <v>0</v>
       </c>
@@ -1625,58 +1624,58 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="25">
-        <v>0</v>
-      </c>
-      <c r="C24" s="25">
-        <v>0</v>
-      </c>
-      <c r="D24" s="25">
-        <v>0</v>
-      </c>
-      <c r="E24" s="25">
-        <v>0</v>
-      </c>
-      <c r="F24" s="25">
-        <v>0</v>
-      </c>
-      <c r="G24" s="25">
-        <v>0</v>
-      </c>
-      <c r="H24" s="25">
+      <c r="B24" s="22">
+        <v>0</v>
+      </c>
+      <c r="C24" s="22">
+        <v>0</v>
+      </c>
+      <c r="D24" s="22">
+        <v>0</v>
+      </c>
+      <c r="E24" s="22">
+        <v>0</v>
+      </c>
+      <c r="F24" s="22">
+        <v>0</v>
+      </c>
+      <c r="G24" s="22">
+        <v>0</v>
+      </c>
+      <c r="H24" s="22">
         <v>141600</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="22">
         <v>206100</v>
       </c>
-      <c r="J24" s="25">
+      <c r="J24" s="22">
         <v>165000</v>
       </c>
-      <c r="K24" s="25">
-        <v>0</v>
-      </c>
-      <c r="L24" s="25">
+      <c r="K24" s="22">
+        <v>0</v>
+      </c>
+      <c r="L24" s="22">
         <f>K24</f>
         <v>0</v>
       </c>
@@ -1684,40 +1683,40 @@
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="25">
-        <v>0</v>
-      </c>
-      <c r="C25" s="25">
-        <v>0</v>
-      </c>
-      <c r="D25" s="25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="25">
-        <v>0</v>
-      </c>
-      <c r="F25" s="25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="25">
-        <v>0</v>
-      </c>
-      <c r="H25" s="25">
+      <c r="B25" s="22">
+        <v>0</v>
+      </c>
+      <c r="C25" s="22">
+        <v>0</v>
+      </c>
+      <c r="D25" s="22">
+        <v>0</v>
+      </c>
+      <c r="E25" s="22">
+        <v>0</v>
+      </c>
+      <c r="F25" s="22">
+        <v>0</v>
+      </c>
+      <c r="G25" s="22">
+        <v>0</v>
+      </c>
+      <c r="H25" s="22">
         <v>472000</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="22">
         <v>687000</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25" s="22">
         <v>550000</v>
       </c>
-      <c r="K25" s="25">
-        <v>0</v>
-      </c>
-      <c r="L25" s="25">
+      <c r="K25" s="22">
+        <v>0</v>
+      </c>
+      <c r="L25" s="22">
         <f>K25</f>
         <v>0</v>
       </c>
@@ -1725,527 +1724,527 @@
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="14">
         <v>0.3</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="14">
         <v>0.31</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="14">
         <v>0.32</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="14">
         <v>0.33</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="14">
         <v>0.33</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="14">
         <v>0.33</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="14">
         <v>0.33</v>
       </c>
-      <c r="I28" s="16">
+      <c r="I28" s="14">
         <v>0.33</v>
       </c>
-      <c r="J28" s="16">
+      <c r="J28" s="14">
         <v>0.33</v>
       </c>
-      <c r="K28" s="16">
+      <c r="K28" s="14">
         <v>0.33</v>
       </c>
-      <c r="L28" s="16">
+      <c r="L28" s="14">
         <v>0.33</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="14">
         <v>0.02</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="14">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D32" s="16">
+      <c r="D32" s="14">
         <v>0.03</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G32" s="16">
+      <c r="G32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="H32" s="16">
+      <c r="H32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I32" s="16">
+      <c r="I32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="J32" s="16">
+      <c r="J32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="K32" s="16">
+      <c r="K32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="L32" s="16">
+      <c r="L32" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="15"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2258,101 +2257,111 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="7">
+      <c r="B1" s="6">
         <v>2025</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="6">
         <v>2026</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="6">
         <v>2027</v>
       </c>
-      <c r="E1" s="7">
+      <c r="E1" s="6">
         <v>2028</v>
       </c>
-      <c r="F1" s="7">
+      <c r="F1" s="6">
         <v>2029</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1" s="6">
         <v>2030</v>
       </c>
-      <c r="H1" s="7">
+      <c r="H1" s="6">
         <v>2031</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="6">
         <v>2032</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J1" s="6">
         <v>2033</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K1" s="6">
         <v>2034</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="6">
         <v>2035</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="23">
         <v>10000</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="19">
-        <v>0</v>
+      <c r="B5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="26"/>
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="23">
+        <v>100000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>